<commit_message>
update to most recent cards code
</commit_message>
<xml_diff>
--- a/inst/extdata/Common_Safety_Displays_cards.xlsx
+++ b/inst/extdata/Common_Safety_Displays_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/ARS_Project/GeneRal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/siera/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="721" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5A90F4A-8574-4656-9720-A56BC19AC03A}"/>
+  <xr:revisionPtr revIDLastSave="743" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01324844-4588-42E0-B415-41645BB2E1AE}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2505" windowWidth="20730" windowHeight="11040" tabRatio="861" firstSheet="1" activeTab="1" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15600" windowHeight="12336" tabRatio="861" firstSheet="19" activeTab="21" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingEvent" sheetId="19" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="620">
   <si>
     <t>id</t>
   </si>
@@ -1940,22 +1940,6 @@
   </si>
   <si>
     <t>groupvar2here</t>
-  </si>
-  <si>
-    <t>df3_analysisidhere &lt;-
-  ard_continuous(
-    data = df2_analysisidhere,
-    by = c(byvarshere),
-    variables = anavarhere
-  ) |&gt;
-mutate(operationid = case_when(stat_name == "N" ~ "Mth02_ContVar_Summ_ByGrp_1_n",
-                                                                     stat_name == "mean" ~ "Mth02_ContVar_Summ_ByGrp_2_Mean",
-                                                                     stat_name == "sd" ~ "Mth02_ContVar_Summ_ByGrp_3_SD",
-                                                                     stat_name == "median" ~ "Mth02_ContVar_Summ_ByGrp_4_Median",
-                                                                     stat_name == "p25" ~ "Mth02_ContVar_Summ_ByGrp_5_Q1",
-                                                                     stat_name == "p75" ~ "Mth02_ContVar_Summ_ByGrp_6_Q3",
-                                                                     stat_name == "min" ~ "Mth02_ContVar_Summ_ByGrp_7_Min",
-                                                                     stat_name == "max" ~ "Mth02_ContVar_Summ_ByGrp_8_Max"))</t>
   </si>
   <si>
     <t>df3_analysisidhere &lt;- 
@@ -2021,9 +2005,6 @@
                                                               stat_name == "p" ~ "Mth01_CatVar_Summ_ByGrp_2_pct"))</t>
   </si>
   <si>
-    <t>bystvarshere</t>
-  </si>
-  <si>
     <t>denom_dataset = df2_denomidhere %&gt;%
   select(denom_anagroupvarshere)
 in_data = df2_analysisidhere %&gt;% 
@@ -2049,9 +2030,6 @@
                                                               stat_name == "p" ~ "Mth01_CatVar_Summ_ByGrp_2_pct"))</t>
   </si>
   <si>
-    <t>stratastvarshere</t>
-  </si>
-  <si>
     <t>strata_vars</t>
   </si>
   <si>
@@ -2062,6 +2040,79 @@
   ) |&gt;
 filter(stat_name == "n")  |&gt;
 mutate(operationid = "Mth01_CatVar_Count_ByGrp_1_n")</t>
+  </si>
+  <si>
+    <t>templateCodeAlt1</t>
+  </si>
+  <si>
+    <t>in_data = df2_analysisidhere |&gt;
+    select(anavarhere, groupvar1here) |&gt;
+    unique()
+df3_analysisidhere &lt;-
+  ard_categorical(
+    data = in_data
+    bystmthere
+  ) |&gt;
+filter(stat_name == 'N') |&gt;
+ mutate(operationid = 'Mth01_CatVar_Count_ByGrp_1_n')</t>
+  </si>
+  <si>
+    <t>denom_dataset = df2_denomanaidhere %&gt;%
+  select(denom_anagroupvarshere)
+in_data = df2_analysisidhere %&gt;% 
+    distinct(distinctlisthere) 
+dataDriven = isdatadrivenhere
+if(dataDriven == TRUE){
+df3_analysisidhere &lt;-
+  ard_categorical(
+    data = in_data
+    stratastmthere,
+    denominator = denom_dataset
+  ) } else {
+df3_analysisidhere &lt;-
+  ard_categorical(
+    data = in_data
+    bystmthere,
+    denominator = denom_dataset
+  ) }
+df3_analysisidhere &lt;- df3_analysisidhere|&gt;
+filter(stat_name %in% c('n', 'p')) |&gt;
+mutate(operationid = case_when(stat_name == 'n' ~ 'Mth01_CatVar_Summ_ByGrp_1_n',
+                                                              stat_name == 'p' ~ 'Mth01_CatVar_Summ_ByGrp_2_pct'))</t>
+  </si>
+  <si>
+    <t>df3_analysisidhere &lt;-
+  ard_continuous(
+    data = df2_analysisidhere,
+    by = c(byvarshere),
+    variables = anavarhere
+  ) |&gt;
+mutate(operationid = case_when(stat_name == 'N' ~ 'Mth02_ContVar_Summ_ByGrp_1_n',
+                                                                     stat_name == 'mean' ~ 'Mth02_ContVar_Summ_ByGrp_2_Mean',
+                                                                     stat_name == 'sd' ~ 'Mth02_ContVar_Summ_ByGrp_3_SD',
+                                                                     stat_name == 'median' ~ 'Mth02_ContVar_Summ_ByGrp_4_Median',
+                                                                     stat_name == 'p25' ~ 'Mth02_ContVar_Summ_ByGrp_5_Q1',
+                                                                     stat_name == 'p75' ~ 'Mth02_ContVar_Summ_ByGrp_6_Q3',
+                                                                     stat_name == 'min' ~ 'Mth02_ContVar_Summ_ByGrp_7_Min',
+                                                                     stat_name == 'max' ~ 'Mth02_ContVar_Summ_ByGrp_8_Max'))</t>
+  </si>
+  <si>
+    <t>df3_analysisidhere &lt;- 
+    ard_stats_chisq_test(by = groupvar1here, data = df2_analysisidhere, variables = groupvar2here)|&gt;
+filter(stat_name == 'p.value') |&gt;
+mutate(operationid = 'Mth03_CatVar_Comp_PChiSq_1_pval')</t>
+  </si>
+  <si>
+    <t>df3_analysisidhere &lt;- 
+    ard_stats_aov(anavarhere ~ groupvar1here, data = df2_analysisidhere) |&gt;
+filter(stat_name == 'p.value') |&gt;
+mutate(operationid = 'Mth04_ContVar_Comp_Anova_1_pval')</t>
+  </si>
+  <si>
+    <t>bystmtvarshere</t>
+  </si>
+  <si>
+    <t>stratastmtvarshere</t>
   </si>
 </sst>
 </file>
@@ -6964,7 +7015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63425975-7444-4301-ABB6-796B2115B6F2}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -7549,10 +7600,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5A7EA2-5BB8-48A0-AE19-CC45569B1AA0}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D7" sqref="A7:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7560,11 +7611,12 @@
     <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="91.109375" customWidth="1"/>
-    <col min="5" max="5" width="48.88671875" customWidth="1"/>
+    <col min="4" max="4" width="93.33203125" customWidth="1"/>
+    <col min="5" max="5" width="91.109375" customWidth="1"/>
+    <col min="6" max="6" width="48.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>91</v>
       </c>
@@ -7578,10 +7630,13 @@
         <v>418</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+        <v>612</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>494</v>
       </c>
@@ -7592,13 +7647,16 @@
         <v>468</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="374.4" x14ac:dyDescent="0.3">
+        <v>611</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>279</v>
       </c>
@@ -7609,13 +7667,16 @@
         <v>468</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>609</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>280</v>
       </c>
@@ -7626,11 +7687,14 @@
         <v>468</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>601</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>615</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>274</v>
       </c>
@@ -7641,10 +7705,13 @@
         <v>468</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>616</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>272</v>
       </c>
@@ -7655,11 +7722,14 @@
         <v>468</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D7" s="6"/>
+        <v>617</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7671,8 +7741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5578B-A7DE-401B-B867-DFECFDE9AF0A}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7735,10 +7805,10 @@
         <v>494</v>
       </c>
       <c r="B4" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="E4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -7782,10 +7852,10 @@
         <v>279</v>
       </c>
       <c r="B8" t="s">
+        <v>603</v>
+      </c>
+      <c r="E8" t="s">
         <v>604</v>
-      </c>
-      <c r="E8" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -7804,10 +7874,10 @@
         <v>279</v>
       </c>
       <c r="B10" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="E10" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -7815,10 +7885,10 @@
         <v>279</v>
       </c>
       <c r="B11" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="E11" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
adding "running interactive" tests
</commit_message>
<xml_diff>
--- a/inst/extdata/Common_Safety_Displays_cards.xlsx
+++ b/inst/extdata/Common_Safety_Displays_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/siera/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="743" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01324844-4588-42E0-B415-41645BB2E1AE}"/>
+  <xr:revisionPtr revIDLastSave="788" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EE34091-5486-4190-B4A5-46318F5CA617}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15600" windowHeight="12336" tabRatio="861" firstSheet="19" activeTab="21" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="861" firstSheet="20" activeTab="20" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingEvent" sheetId="19" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="629">
   <si>
     <t>id</t>
   </si>
@@ -1903,9 +1903,6 @@
     <t>AG_var2</t>
   </si>
   <si>
-    <t>string for "by" and "variables" parameter for the ard_categorical function with bigN only</t>
-  </si>
-  <si>
     <t>string for "by" and "variables" parameter for the ard_continuous function</t>
   </si>
   <si>
@@ -1916,9 +1913,6 @@
   </si>
   <si>
     <t>by_listc</t>
-  </si>
-  <si>
-    <t>denomidhere</t>
   </si>
   <si>
     <t>anavarhere</t>
@@ -2045,42 +2039,6 @@
     <t>templateCodeAlt1</t>
   </si>
   <si>
-    <t>in_data = df2_analysisidhere |&gt;
-    select(anavarhere, groupvar1here) |&gt;
-    unique()
-df3_analysisidhere &lt;-
-  ard_categorical(
-    data = in_data
-    bystmthere
-  ) |&gt;
-filter(stat_name == 'N') |&gt;
- mutate(operationid = 'Mth01_CatVar_Count_ByGrp_1_n')</t>
-  </si>
-  <si>
-    <t>denom_dataset = df2_denomanaidhere %&gt;%
-  select(denom_anagroupvarshere)
-in_data = df2_analysisidhere %&gt;% 
-    distinct(distinctlisthere) 
-dataDriven = isdatadrivenhere
-if(dataDriven == TRUE){
-df3_analysisidhere &lt;-
-  ard_categorical(
-    data = in_data
-    stratastmthere,
-    denominator = denom_dataset
-  ) } else {
-df3_analysisidhere &lt;-
-  ard_categorical(
-    data = in_data
-    bystmthere,
-    denominator = denom_dataset
-  ) }
-df3_analysisidhere &lt;- df3_analysisidhere|&gt;
-filter(stat_name %in% c('n', 'p')) |&gt;
-mutate(operationid = case_when(stat_name == 'n' ~ 'Mth01_CatVar_Summ_ByGrp_1_n',
-                                                              stat_name == 'p' ~ 'Mth01_CatVar_Summ_ByGrp_2_pct'))</t>
-  </si>
-  <si>
     <t>df3_analysisidhere &lt;-
   ard_continuous(
     data = df2_analysisidhere,
@@ -2097,22 +2055,104 @@
                                                                      stat_name == 'max' ~ 'Mth02_ContVar_Summ_ByGrp_8_Max'))</t>
   </si>
   <si>
+    <t>bystmthere</t>
+  </si>
+  <si>
+    <t>stratastmthere</t>
+  </si>
+  <si>
+    <t>Analysis variable to be summarised</t>
+  </si>
+  <si>
+    <t>Analysis grouping variable from Group1</t>
+  </si>
+  <si>
+    <t>"by = " and "variable = " statements for ard_tabulate() with dynamic variables</t>
+  </si>
+  <si>
+    <t>"strata =  and "variable = " statements for ard_tabulate() with dynamic variables</t>
+  </si>
+  <si>
+    <t>"by =  and "variable = " statements for ard_tabulate() with dynamic variables</t>
+  </si>
+  <si>
+    <t>denomanaidhere</t>
+  </si>
+  <si>
+    <t>Analysis ID for Denominator Analysis</t>
+  </si>
+  <si>
+    <t>Analysis Grouping variables for denominator dataset</t>
+  </si>
+  <si>
+    <t>dataDriven boolean value for highest Analysisgrouping factor</t>
+  </si>
+  <si>
+    <t>Analysis grouping variable from Group2</t>
+  </si>
+  <si>
+    <t>in_data = df2_analysisidhere |&gt;
+    dplyr::select(anavarhere, groupvar1here) |&gt;
+    unique()
+df3_analysisidhere &lt;-
+  cards::ard_categorical(
+    data = in_data
+    bystmthere
+  ) |&gt;
+dplyr::filter(stat_name == 'N') |&gt;
+ dplyr::mutate(operationid = 'Mth01_CatVar_Count_ByGrp_1_n')</t>
+  </si>
+  <si>
+    <t>denom_dataset = df2_denomanaidhere |&gt;
+  dplyr::select(denom_anagroupvarshere)
+in_data = df2_analysisidhere |&gt;
+    dplyr::distinct(distinctlisthere) 
+dataDriven = isdatadrivenhere
+if(dataDriven == TRUE){
+df3_analysisidhere &lt;-
+  cards::ard_categorical(
+    data = in_data
+    stratastmthere,
+    denominator = denom_dataset
+  ) } else {
+df3_analysisidhere &lt;-
+  cards::ard_categorical(
+    data = in_data
+    bystmthere,
+    denominator = denom_dataset
+  ) }
+df3_analysisidhere &lt;- df3_analysisidhere|&gt;
+dplyr::filter(stat_name %in% c('n', 'p')) |&gt;
+dplyr::mutate(operationid = dplyr::case_when(stat_name == 'n' ~ 'Mth01_CatVar_Summ_ByGrp_1_n',
+                                                              stat_name == 'p' ~ 'Mth01_CatVar_Summ_ByGrp_2_pct'))</t>
+  </si>
+  <si>
+    <t>df3_analysisidhere &lt;-
+  cards::ard_continuous(
+    data = df2_analysisidhere,
+    by = c(byvarshere),
+    variables = anavarhere
+  ) |&gt;
+dplyr::mutate(operationid = dplyr::case_when(stat_name == 'N' ~ 'Mth02_ContVar_Summ_ByGrp_1_n',
+                                                                     stat_name == 'mean' ~ 'Mth02_ContVar_Summ_ByGrp_2_Mean',
+                                                                     stat_name == 'sd' ~ 'Mth02_ContVar_Summ_ByGrp_3_SD',
+                                                                     stat_name == 'median' ~ 'Mth02_ContVar_Summ_ByGrp_4_Median',
+                                                                     stat_name == 'p25' ~ 'Mth02_ContVar_Summ_ByGrp_5_Q1',
+                                                                     stat_name == 'p75' ~ 'Mth02_ContVar_Summ_ByGrp_6_Q3',
+                                                                     stat_name == 'min' ~ 'Mth02_ContVar_Summ_ByGrp_7_Min',
+                                                                     stat_name == 'max' ~ 'Mth02_ContVar_Summ_ByGrp_8_Max'))</t>
+  </si>
+  <si>
     <t>df3_analysisidhere &lt;- 
-    ard_stats_chisq_test(by = groupvar1here, data = df2_analysisidhere, variables = groupvar2here)|&gt;
-filter(stat_name == 'p.value') |&gt;
-mutate(operationid = 'Mth03_CatVar_Comp_PChiSq_1_pval')</t>
+    cardx::ard_stats_chisq_test(by = groupvar1here, data = df2_analysisidhere, variables = groupvar2here)|&gt;
+dplyr::filter(stat_name == 'p.value') |&gt;
+dplyr::mutate(operationid = 'Mth03_CatVar_Comp_PChiSq_1_pval')</t>
   </si>
   <si>
     <t>df3_analysisidhere &lt;- 
-    ard_stats_aov(anavarhere ~ groupvar1here, data = df2_analysisidhere) |&gt;
-filter(stat_name == 'p.value') |&gt;
-mutate(operationid = 'Mth04_ContVar_Comp_Anova_1_pval')</t>
-  </si>
-  <si>
-    <t>bystmtvarshere</t>
-  </si>
-  <si>
-    <t>stratastmtvarshere</t>
+    cardx::ard_stats_aov(anavarhere ~ groupvar1here, data = df2_analysisidhere) |&gt;
+dplyr::filter(stat_name == 'p.value') |&gt;
+dplyr::mutate(operationid = 'Mth04_ContVar_Comp_Anova_1_pval')</t>
   </si>
 </sst>
 </file>
@@ -7602,7 +7642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5A7EA2-5BB8-48A0-AE19-CC45569B1AA0}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -7630,10 +7670,10 @@
         <v>418</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
@@ -7647,13 +7687,13 @@
         <v>468</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>613</v>
+        <v>624</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
@@ -7667,13 +7707,13 @@
         <v>468</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>614</v>
+        <v>625</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
@@ -7687,10 +7727,10 @@
         <v>468</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>615</v>
+        <v>626</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -7705,10 +7745,10 @@
         <v>468</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>616</v>
+        <v>627</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -7722,10 +7762,10 @@
         <v>468</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>617</v>
+        <v>628</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -7739,10 +7779,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5578B-A7DE-401B-B867-DFECFDE9AF0A}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7780,13 +7820,13 @@
         <v>494</v>
       </c>
       <c r="B2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C2" t="s">
-        <v>588</v>
+        <v>614</v>
       </c>
       <c r="E2" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -7794,10 +7834,13 @@
         <v>494</v>
       </c>
       <c r="B3" t="s">
-        <v>594</v>
+        <v>597</v>
+      </c>
+      <c r="C3" t="s">
+        <v>615</v>
       </c>
       <c r="E3" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -7805,10 +7848,13 @@
         <v>494</v>
       </c>
       <c r="B4" t="s">
-        <v>618</v>
+        <v>612</v>
+      </c>
+      <c r="C4" t="s">
+        <v>616</v>
       </c>
       <c r="E4" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -7816,13 +7862,13 @@
         <v>279</v>
       </c>
       <c r="B5" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -7830,7 +7876,10 @@
         <v>279</v>
       </c>
       <c r="B6" t="s">
-        <v>593</v>
+        <v>619</v>
+      </c>
+      <c r="C6" t="s">
+        <v>620</v>
       </c>
       <c r="E6" t="s">
         <v>586</v>
@@ -7841,10 +7890,13 @@
         <v>279</v>
       </c>
       <c r="B7" t="s">
-        <v>596</v>
+        <v>594</v>
+      </c>
+      <c r="C7" t="s">
+        <v>621</v>
       </c>
       <c r="E7" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -7852,10 +7904,13 @@
         <v>279</v>
       </c>
       <c r="B8" t="s">
-        <v>603</v>
+        <v>601</v>
+      </c>
+      <c r="C8" t="s">
+        <v>622</v>
       </c>
       <c r="E8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -7863,10 +7918,13 @@
         <v>279</v>
       </c>
       <c r="B9" t="s">
-        <v>595</v>
+        <v>612</v>
+      </c>
+      <c r="C9" t="s">
+        <v>618</v>
       </c>
       <c r="E9" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -7874,21 +7932,27 @@
         <v>279</v>
       </c>
       <c r="B10" t="s">
-        <v>618</v>
+        <v>613</v>
+      </c>
+      <c r="C10" t="s">
+        <v>617</v>
       </c>
       <c r="E10" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B11" t="s">
-        <v>619</v>
+        <v>593</v>
+      </c>
+      <c r="C11" t="s">
+        <v>588</v>
       </c>
       <c r="E11" t="s">
-        <v>610</v>
+        <v>591</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -7896,24 +7960,27 @@
         <v>280</v>
       </c>
       <c r="B12" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C12" t="s">
-        <v>589</v>
+        <v>614</v>
       </c>
       <c r="E12" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B13" t="s">
-        <v>594</v>
+        <v>597</v>
+      </c>
+      <c r="C13" t="s">
+        <v>615</v>
       </c>
       <c r="E13" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -7921,21 +7988,27 @@
         <v>274</v>
       </c>
       <c r="B14" t="s">
-        <v>599</v>
+        <v>598</v>
+      </c>
+      <c r="C14" t="s">
+        <v>623</v>
       </c>
       <c r="E14" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B15" t="s">
-        <v>600</v>
+        <v>592</v>
+      </c>
+      <c r="C15" t="s">
+        <v>614</v>
       </c>
       <c r="E15" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -7943,20 +8016,12 @@
         <v>272</v>
       </c>
       <c r="B16" t="s">
-        <v>594</v>
+        <v>597</v>
+      </c>
+      <c r="C16" t="s">
+        <v>615</v>
       </c>
       <c r="E16" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>272</v>
-      </c>
-      <c r="B17" t="s">
-        <v>599</v>
-      </c>
-      <c r="E17" t="s">
         <v>585</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add tests for xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/Common_Safety_Displays_cards.xlsx
+++ b/inst/extdata/Common_Safety_Displays_cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/siera/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="788" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EE34091-5486-4190-B4A5-46318F5CA617}"/>
+  <xr:revisionPtr revIDLastSave="789" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98D31A30-A1B2-4276-A400-F431A1153DBF}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="861" firstSheet="20" activeTab="20" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="747" firstSheet="15" activeTab="15" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingEvent" sheetId="19" r:id="rId1"/>
@@ -2091,18 +2091,6 @@
     <t>Analysis grouping variable from Group2</t>
   </si>
   <si>
-    <t>in_data = df2_analysisidhere |&gt;
-    dplyr::select(anavarhere, groupvar1here) |&gt;
-    unique()
-df3_analysisidhere &lt;-
-  cards::ard_categorical(
-    data = in_data
-    bystmthere
-  ) |&gt;
-dplyr::filter(stat_name == 'N') |&gt;
- dplyr::mutate(operationid = 'Mth01_CatVar_Count_ByGrp_1_n')</t>
-  </si>
-  <si>
     <t>denom_dataset = df2_denomanaidhere |&gt;
   dplyr::select(denom_anagroupvarshere)
 in_data = df2_analysisidhere |&gt;
@@ -2153,6 +2141,18 @@
     cardx::ard_stats_aov(anavarhere ~ groupvar1here, data = df2_analysisidhere) |&gt;
 dplyr::filter(stat_name == 'p.value') |&gt;
 dplyr::mutate(operationid = 'Mth04_ContVar_Comp_Anova_1_pval')</t>
+  </si>
+  <si>
+    <t>in_data = df2_analysisidhere |&gt;
+    dplyr::select(anavarhere, groupvar1here) |&gt;
+    unique()
+df3_analysisidhere &lt;-
+  cards::ard_categorical(
+    data = in_data
+    bystmthere
+  ) |&gt;
+dplyr::filter(stat_name == 'n') |&gt;
+ dplyr::mutate(operationid = 'Mth01_CatVar_Count_ByGrp_1_n')</t>
   </si>
 </sst>
 </file>
@@ -5094,8 +5094,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7642,8 +7642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5A7EA2-5BB8-48A0-AE19-CC45569B1AA0}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7687,7 +7687,7 @@
         <v>468</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>609</v>
@@ -7707,7 +7707,7 @@
         <v>468</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>606</v>
@@ -7727,7 +7727,7 @@
         <v>468</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>611</v>
@@ -7745,7 +7745,7 @@
         <v>468</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>599</v>
@@ -7762,7 +7762,7 @@
         <v>468</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>600</v>

</xml_diff>

<commit_message>
make dynamic data subset dataset assignments
</commit_message>
<xml_diff>
--- a/inst/extdata/Common_Safety_Displays_cards.xlsx
+++ b/inst/extdata/Common_Safety_Displays_cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/siera/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="789" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98D31A30-A1B2-4276-A400-F431A1153DBF}"/>
+  <xr:revisionPtr revIDLastSave="799" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C84A3159-A12C-4EE9-9DB3-F7EB28FB06A5}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="747" firstSheet="15" activeTab="15" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="747" firstSheet="17" activeTab="21" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingEvent" sheetId="19" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="630">
   <si>
     <t>id</t>
   </si>
@@ -2153,6 +2153,33 @@
   ) |&gt;
 dplyr::filter(stat_name == 'n') |&gt;
  dplyr::mutate(operationid = 'Mth01_CatVar_Count_ByGrp_1_n')</t>
+  </si>
+  <si>
+    <t>denom_dataset = df2_denomanaidhere |&gt;
+  dplyr::select(denom_anagroupvarshere)
+in_data = df2_analysisidhere |&gt;
+    dplyr::distinct(distinctlisthere) |&gt;
+    dplyr::mutate(dummy = 'dummyvar')
+dataDriven = isdatadrivenhere
+if(dataDriven == TRUE){
+df3_analysisidhere &lt;-
+  cards::ard_categorical(
+    data = in_data,
+    strata = c(byvarshere),
+    variables = 'dummy',
+    denominator = denom_dataset
+  ) } else {
+df3_analysisidhere &lt;-
+ cards::ard_categorical(
+    data = in_data,
+    by = c(byvarshere),
+    variables = 'dummy',
+    denominator = denom_dataset
+  ) }
+df3_analysisidhere &lt;- df3_analysisidhere|&gt;
+dplyr::filter(stat_name %in% c('n', 'p')) |&gt;
+dplyr::mutate(operationid = dplyr::case_when(stat_name == 'n' ~ 'Mth01_CatVar_Summ_ByGrp_1_n',
+                                                              stat_name == 'p' ~ 'Mth01_CatVar_Summ_ByGrp_2_pct'))</t>
   </si>
 </sst>
 </file>
@@ -2188,7 +2215,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2198,6 +2225,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2214,7 +2247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -2228,6 +2261,9 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5094,7 +5130,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
@@ -7640,9 +7676,9 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5A7EA2-5BB8-48A0-AE19-CC45569B1AA0}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -7654,9 +7690,10 @@
     <col min="4" max="4" width="93.33203125" customWidth="1"/>
     <col min="5" max="5" width="91.109375" customWidth="1"/>
     <col min="6" max="6" width="48.88671875" customWidth="1"/>
+    <col min="7" max="7" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>91</v>
       </c>
@@ -7676,7 +7713,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>494</v>
       </c>
@@ -7696,7 +7733,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>279</v>
       </c>
@@ -7706,8 +7743,8 @@
       <c r="C3" t="s">
         <v>468</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>624</v>
+      <c r="D3" s="7" t="s">
+        <v>629</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>606</v>
@@ -7715,8 +7752,11 @@
       <c r="F3" s="6" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="G3" s="6" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>280</v>
       </c>
@@ -7734,7 +7774,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>274</v>
       </c>
@@ -7751,7 +7791,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>272</v>
       </c>
@@ -7768,7 +7808,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E7" s="6"/>
     </row>
   </sheetData>
@@ -7779,10 +7819,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5578B-A7DE-401B-B867-DFECFDE9AF0A}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7943,7 +7983,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B11" t="s">
         <v>593</v>
@@ -7960,27 +8000,27 @@
         <v>280</v>
       </c>
       <c r="B12" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C12" t="s">
-        <v>614</v>
+        <v>588</v>
       </c>
       <c r="E12" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B13" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="C13" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E13" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -7988,27 +8028,27 @@
         <v>274</v>
       </c>
       <c r="B14" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C14" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="E14" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B15" t="s">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="C15" t="s">
-        <v>614</v>
+        <v>623</v>
       </c>
       <c r="E15" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -8016,12 +8056,26 @@
         <v>272</v>
       </c>
       <c r="B16" t="s">
+        <v>592</v>
+      </c>
+      <c r="C16" t="s">
+        <v>614</v>
+      </c>
+      <c r="E16" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" t="s">
         <v>597</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>615</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>585</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed extra column in AMCT
</commit_message>
<xml_diff>
--- a/inst/extdata/Common_Safety_Displays_cards.xlsx
+++ b/inst/extdata/Common_Safety_Displays_cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/siera/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="799" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C84A3159-A12C-4EE9-9DB3-F7EB28FB06A5}"/>
+  <xr:revisionPtr revIDLastSave="800" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{552B6B97-8026-47B0-B26D-B4D358F22BC2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="747" firstSheet="17" activeTab="21" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="747" firstSheet="16" activeTab="20" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingEvent" sheetId="19" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="629">
   <si>
     <t>id</t>
   </si>
@@ -1992,31 +1992,6 @@
     by = c(byvarshere),
     variables = 'dummy',
     denominator = denom_dataset
-  ) }
-df3_analysisidhere &lt;- df3_analysisidhere|&gt;
-filter(stat_name %in% c("n", "p")) |&gt;
-mutate(operationid = case_when(stat_name == "n" ~ "Mth01_CatVar_Summ_ByGrp_1_n",
-                                                              stat_name == "p" ~ "Mth01_CatVar_Summ_ByGrp_2_pct"))</t>
-  </si>
-  <si>
-    <t>denom_dataset = df2_denomidhere %&gt;%
-  select(denom_anagroupvarshere)
-in_data = df2_analysisidhere %&gt;% 
-    distinct(distinctlisthere) %&gt;%
-    mutate(dummy = "dummyvar")
-dataDriven = isdatadrivenhere
-if(dataDriven == TRUE){
-df3_analysisidhere &lt;-
-  ard_categorical(
-    data = in_data
-    stratastvarshere
-    ,denominator = denom_dataset
-  ) } else {
-df3_analysisidhere &lt;-
-  ard_categorical(
-    data = in_data
-    bystvarshere
-    ,denominator = denom_dataset
   ) }
 df3_analysisidhere &lt;- df3_analysisidhere|&gt;
 filter(stat_name %in% c("n", "p")) |&gt;
@@ -7676,10 +7651,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5A7EA2-5BB8-48A0-AE19-CC45569B1AA0}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7693,7 +7668,7 @@
     <col min="7" max="7" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>91</v>
       </c>
@@ -7707,13 +7682,13 @@
         <v>418</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>494</v>
       </c>
@@ -7724,16 +7699,16 @@
         <v>468</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>279</v>
       </c>
@@ -7744,19 +7719,16 @@
         <v>468</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>606</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>607</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>280</v>
       </c>
@@ -7767,14 +7739,14 @@
         <v>468</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>274</v>
       </c>
@@ -7785,13 +7757,13 @@
         <v>468</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>272</v>
       </c>
@@ -7802,13 +7774,13 @@
         <v>468</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E7" s="6"/>
     </row>
   </sheetData>
@@ -7821,7 +7793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5578B-A7DE-401B-B867-DFECFDE9AF0A}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -7863,7 +7835,7 @@
         <v>592</v>
       </c>
       <c r="C2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E2" t="s">
         <v>584</v>
@@ -7877,7 +7849,7 @@
         <v>597</v>
       </c>
       <c r="C3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E3" t="s">
         <v>585</v>
@@ -7888,10 +7860,10 @@
         <v>494</v>
       </c>
       <c r="B4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E4" t="s">
         <v>603</v>
@@ -7916,10 +7888,10 @@
         <v>279</v>
       </c>
       <c r="B6" t="s">
+        <v>618</v>
+      </c>
+      <c r="C6" t="s">
         <v>619</v>
-      </c>
-      <c r="C6" t="s">
-        <v>620</v>
       </c>
       <c r="E6" t="s">
         <v>586</v>
@@ -7933,7 +7905,7 @@
         <v>594</v>
       </c>
       <c r="C7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E7" t="s">
         <v>595</v>
@@ -7947,7 +7919,7 @@
         <v>601</v>
       </c>
       <c r="C8" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E8" t="s">
         <v>602</v>
@@ -7958,10 +7930,10 @@
         <v>279</v>
       </c>
       <c r="B9" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C9" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E9" t="s">
         <v>603</v>
@@ -7972,13 +7944,13 @@
         <v>279</v>
       </c>
       <c r="B10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -8017,7 +7989,7 @@
         <v>592</v>
       </c>
       <c r="C13" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E13" t="s">
         <v>584</v>
@@ -8031,7 +8003,7 @@
         <v>597</v>
       </c>
       <c r="C14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E14" t="s">
         <v>585</v>
@@ -8045,7 +8017,7 @@
         <v>598</v>
       </c>
       <c r="C15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E15" t="s">
         <v>587</v>
@@ -8059,7 +8031,7 @@
         <v>592</v>
       </c>
       <c r="C16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E16" t="s">
         <v>584</v>
@@ -8073,7 +8045,7 @@
         <v>597</v>
       </c>
       <c r="C17" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E17" t="s">
         <v>585</v>
@@ -8536,8 +8508,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
handle groupings and completed LOPA
</commit_message>
<xml_diff>
--- a/inst/extdata/Common_Safety_Displays_cards.xlsx
+++ b/inst/extdata/Common_Safety_Displays_cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/siera/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="800" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{552B6B97-8026-47B0-B26D-B4D358F22BC2}"/>
+  <xr:revisionPtr revIDLastSave="801" documentId="13_ncr:1_{65D881D3-B504-42B3-944D-AEE34ED84ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F1B20F9-DBE0-4E31-9AAB-8A6CF14CAE35}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="747" firstSheet="16" activeTab="20" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="747" firstSheet="16" activeTab="20" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingEvent" sheetId="19" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="620">
   <si>
     <t>id</t>
   </si>
@@ -1936,18 +1936,6 @@
     <t>groupvar2here</t>
   </si>
   <si>
-    <t>df3_analysisidhere &lt;- 
-    ard_stats_chisq_test(by = groupvar1here, data = df2_analysisidhere, variables = groupvar2here)|&gt;
-filter(stat_name == "p.value") |&gt;
-mutate(operationid = "Mth03_CatVar_Comp_PChiSq_1_pval")</t>
-  </si>
-  <si>
-    <t>df3_analysisidhere &lt;- 
-    ard_stats_aov(anavarhere ~ groupvar1here, data = df2_analysisidhere) |&gt;
-filter(stat_name == "p.value") |&gt;
-mutate(operationid = "Mth04_ContVar_Comp_Anova_1_pval")</t>
-  </si>
-  <si>
     <t>isdatadrivenhere</t>
   </si>
   <si>
@@ -1957,79 +1945,9 @@
     <t>by_vars</t>
   </si>
   <si>
-    <t>templateCode_alt</t>
-  </si>
-  <si>
-    <t>df3_analysisidhere &lt;-
-  ard_categorical(
-    data = df2_analysisidhere
-    by = byvarshere,
-    variables = anavarhere
-  ) |&gt;
-filter(stat_name == "N") |&gt;
-select(-variable, -variable_level) |&gt;
-unique() |&gt;
-mutate(operationid = "Mth01_CatVar_Count_ByGrp_1_n")</t>
-  </si>
-  <si>
-    <t>denom_dataset = df2_denomidhere %&gt;%
-  select(denom_anagroupvarshere)
-in_data = df2_analysisidhere %&gt;% 
-    distinct(distinctlisthere) %&gt;%
-    mutate(dummy = "dummyvar")
-dataDriven = isdatadrivenhere
-if(dataDriven == TRUE){
-df3_analysisidhere &lt;-
-  ard_categorical(
-    data = in_data,
-    strata = c(byvarshere),
-    variables = 'dummy',
-    denominator = denom_dataset
-  ) } else {
-df3_analysisidhere &lt;-
-  ard_categorical(
-    data = in_data,
-    by = c(byvarshere),
-    variables = 'dummy',
-    denominator = denom_dataset
-  ) }
-df3_analysisidhere &lt;- df3_analysisidhere|&gt;
-filter(stat_name %in% c("n", "p")) |&gt;
-mutate(operationid = case_when(stat_name == "n" ~ "Mth01_CatVar_Summ_ByGrp_1_n",
-                                                              stat_name == "p" ~ "Mth01_CatVar_Summ_ByGrp_2_pct"))</t>
-  </si>
-  <si>
     <t>strata_vars</t>
   </si>
   <si>
-    <t>df3_analysisidhere &lt;-
-  ard_categorical(
-    data = df2_analysisidhere
-    bystvarshere
-  ) |&gt;
-filter(stat_name == "n")  |&gt;
-mutate(operationid = "Mth01_CatVar_Count_ByGrp_1_n")</t>
-  </si>
-  <si>
-    <t>templateCodeAlt1</t>
-  </si>
-  <si>
-    <t>df3_analysisidhere &lt;-
-  ard_continuous(
-    data = df2_analysisidhere,
-    by = c(byvarshere),
-    variables = anavarhere
-  ) |&gt;
-mutate(operationid = case_when(stat_name == 'N' ~ 'Mth02_ContVar_Summ_ByGrp_1_n',
-                                                                     stat_name == 'mean' ~ 'Mth02_ContVar_Summ_ByGrp_2_Mean',
-                                                                     stat_name == 'sd' ~ 'Mth02_ContVar_Summ_ByGrp_3_SD',
-                                                                     stat_name == 'median' ~ 'Mth02_ContVar_Summ_ByGrp_4_Median',
-                                                                     stat_name == 'p25' ~ 'Mth02_ContVar_Summ_ByGrp_5_Q1',
-                                                                     stat_name == 'p75' ~ 'Mth02_ContVar_Summ_ByGrp_6_Q3',
-                                                                     stat_name == 'min' ~ 'Mth02_ContVar_Summ_ByGrp_7_Min',
-                                                                     stat_name == 'max' ~ 'Mth02_ContVar_Summ_ByGrp_8_Max'))</t>
-  </si>
-  <si>
     <t>bystmthere</t>
   </si>
   <si>
@@ -2064,30 +1982,6 @@
   </si>
   <si>
     <t>Analysis grouping variable from Group2</t>
-  </si>
-  <si>
-    <t>denom_dataset = df2_denomanaidhere |&gt;
-  dplyr::select(denom_anagroupvarshere)
-in_data = df2_analysisidhere |&gt;
-    dplyr::distinct(distinctlisthere) 
-dataDriven = isdatadrivenhere
-if(dataDriven == TRUE){
-df3_analysisidhere &lt;-
-  cards::ard_categorical(
-    data = in_data
-    stratastmthere,
-    denominator = denom_dataset
-  ) } else {
-df3_analysisidhere &lt;-
-  cards::ard_categorical(
-    data = in_data
-    bystmthere,
-    denominator = denom_dataset
-  ) }
-df3_analysisidhere &lt;- df3_analysisidhere|&gt;
-dplyr::filter(stat_name %in% c('n', 'p')) |&gt;
-dplyr::mutate(operationid = dplyr::case_when(stat_name == 'n' ~ 'Mth01_CatVar_Summ_ByGrp_1_n',
-                                                              stat_name == 'p' ~ 'Mth01_CatVar_Summ_ByGrp_2_pct'))</t>
   </si>
   <si>
     <t>df3_analysisidhere &lt;-
@@ -7653,8 +7547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5A7EA2-5BB8-48A0-AE19-CC45569B1AA0}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7681,14 +7575,10 @@
       <c r="D1" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>494</v>
       </c>
@@ -7699,14 +7589,10 @@
         <v>468</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>627</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>605</v>
-      </c>
+        <v>618</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -7719,14 +7605,10 @@
         <v>468</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>628</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>606</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>623</v>
-      </c>
+        <v>619</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -7739,11 +7621,9 @@
         <v>468</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>624</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>610</v>
-      </c>
+        <v>615</v>
+      </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -7757,11 +7637,9 @@
         <v>468</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>625</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>599</v>
-      </c>
+        <v>616</v>
+      </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -7774,11 +7652,9 @@
         <v>468</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>626</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>600</v>
-      </c>
+        <v>617</v>
+      </c>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E7" s="6"/>
@@ -7835,7 +7711,7 @@
         <v>592</v>
       </c>
       <c r="C2" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="E2" t="s">
         <v>584</v>
@@ -7849,7 +7725,7 @@
         <v>597</v>
       </c>
       <c r="C3" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="E3" t="s">
         <v>585</v>
@@ -7860,13 +7736,13 @@
         <v>494</v>
       </c>
       <c r="B4" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="C4" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="E4" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -7888,10 +7764,10 @@
         <v>279</v>
       </c>
       <c r="B6" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="C6" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="E6" t="s">
         <v>586</v>
@@ -7905,7 +7781,7 @@
         <v>594</v>
       </c>
       <c r="C7" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="E7" t="s">
         <v>595</v>
@@ -7916,13 +7792,13 @@
         <v>279</v>
       </c>
       <c r="B8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C8" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="E8" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -7930,13 +7806,13 @@
         <v>279</v>
       </c>
       <c r="B9" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="C9" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="E9" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -7944,13 +7820,13 @@
         <v>279</v>
       </c>
       <c r="B10" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="C10" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="E10" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -7989,7 +7865,7 @@
         <v>592</v>
       </c>
       <c r="C13" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="E13" t="s">
         <v>584</v>
@@ -8003,7 +7879,7 @@
         <v>597</v>
       </c>
       <c r="C14" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="E14" t="s">
         <v>585</v>
@@ -8017,7 +7893,7 @@
         <v>598</v>
       </c>
       <c r="C15" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="E15" t="s">
         <v>587</v>
@@ -8031,7 +7907,7 @@
         <v>592</v>
       </c>
       <c r="C16" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="E16" t="s">
         <v>584</v>
@@ -8045,7 +7921,7 @@
         <v>597</v>
       </c>
       <c r="C17" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="E17" t="s">
         <v>585</v>

</xml_diff>